<commit_message>
updated test case name
</commit_message>
<xml_diff>
--- a/Applause_Assignment/src/test/resources/data/Applause_Products.xlsx
+++ b/Applause_Assignment/src/test/resources/data/Applause_Products.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="109">
   <si>
     <t>Highlights</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>44</t>
+  </si>
+  <si>
+    <t>43</t>
   </si>
 </sst>
 </file>
@@ -760,32 +763,32 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
@@ -795,12 +798,12 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
@@ -815,17 +818,17 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>20</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23">
@@ -835,17 +838,17 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27">
@@ -855,17 +858,17 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
@@ -880,87 +883,87 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50">
@@ -970,12 +973,12 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53">
@@ -985,12 +988,12 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1105,12 +1108,12 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
@@ -1392,12 +1395,12 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
@@ -1457,12 +1460,12 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33">
@@ -2246,7 +2249,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
@@ -2609,57 +2612,57 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>20</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22">
@@ -2669,77 +2672,77 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
@@ -2749,22 +2752,22 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -2774,42 +2777,42 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3200,12 +3203,12 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
@@ -3265,12 +3268,12 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33">
@@ -3487,12 +3490,12 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
@@ -3552,12 +3555,12 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33">

</xml_diff>

<commit_message>
updated all the configs
</commit_message>
<xml_diff>
--- a/Applause_Assignment/src/test/resources/data/Applause_Products.xlsx
+++ b/Applause_Assignment/src/test/resources/data/Applause_Products.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5145" uniqueCount="112">
   <si>
     <t>Highlights</t>
   </si>
@@ -354,6 +354,15 @@
   </si>
   <si>
     <t>43</t>
+  </si>
+  <si>
+    <t>SOL DE JANEIRO</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>CHOPARD</t>
   </si>
 </sst>
 </file>
@@ -763,32 +772,32 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -798,37 +807,37 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>84</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
@@ -838,17 +847,17 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
@@ -858,112 +867,112 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50">
@@ -973,12 +982,12 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53">
@@ -988,12 +997,12 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1128,42 +1137,42 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>25</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30">
@@ -1173,97 +1182,97 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>97</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>98</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50">
@@ -1273,27 +1282,27 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>100</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1930,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2224,7 +2233,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:C51"/>
+  <dimension ref="A2:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2249,7 +2258,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -2321,47 +2330,47 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>39</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>25</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26">
@@ -2371,92 +2380,92 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>97</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>97</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>98</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45">
@@ -2466,32 +2475,52 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>100</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>71</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>71</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2612,57 +2641,57 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>84</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22">
@@ -2672,77 +2701,77 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
@@ -2752,22 +2781,22 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43">
@@ -2777,42 +2806,42 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3203,12 +3232,12 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
@@ -3243,27 +3272,27 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>43</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31">
@@ -3278,117 +3307,117 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -4233,102 +4262,102 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>74</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>82</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>19</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>44</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>87</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>28</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40">
@@ -4338,7 +4367,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>89</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
@@ -4348,7 +4377,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44">
@@ -4363,42 +4392,42 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>25</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>